<commit_message>
Updated first sprint start date
</commit_message>
<xml_diff>
--- a/webshop_agile_gantt.xlsx
+++ b/webshop_agile_gantt.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB53CAE-B05B-4813-971C-4560B691E7C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F936EFBA-A814-40B0-BBE0-C14A5B455894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21840" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1990,8 +1990,8 @@
   </sheetPr>
   <dimension ref="A1:BR37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="B1" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="X12" sqref="X12"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -3051,7 +3051,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="29">
-        <v>45200</v>
+        <v>45201</v>
       </c>
       <c r="G10" s="30">
         <v>14</v>
@@ -3298,7 +3298,7 @@
       </c>
       <c r="F11" s="29">
         <f>F10+14</f>
-        <v>45214</v>
+        <v>45215</v>
       </c>
       <c r="G11" s="30">
         <v>14</v>
@@ -3545,7 +3545,7 @@
       </c>
       <c r="F12" s="29">
         <f t="shared" ref="F12:F15" si="10">F11+14</f>
-        <v>45228</v>
+        <v>45229</v>
       </c>
       <c r="G12" s="30">
         <v>14</v>
@@ -3792,7 +3792,7 @@
       </c>
       <c r="F13" s="29">
         <f t="shared" si="10"/>
-        <v>45242</v>
+        <v>45243</v>
       </c>
       <c r="G13" s="30">
         <v>14</v>
@@ -4039,7 +4039,7 @@
       </c>
       <c r="F14" s="29">
         <f t="shared" si="10"/>
-        <v>45256</v>
+        <v>45257</v>
       </c>
       <c r="G14" s="30">
         <v>14</v>
@@ -4286,7 +4286,7 @@
       </c>
       <c r="F15" s="29">
         <f t="shared" si="10"/>
-        <v>45270</v>
+        <v>45271</v>
       </c>
       <c r="G15" s="30">
         <v>14</v>

</xml_diff>

<commit_message>
Updated Sprint Gantt Chart
</commit_message>
<xml_diff>
--- a/webshop_agile_gantt.xlsx
+++ b/webshop_agile_gantt.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F936EFBA-A814-40B0-BBE0-C14A5B455894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD5996D9-D3EA-4CF9-83B0-F62A71E5AABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21840" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1991,7 +1991,7 @@
   <dimension ref="A1:BR37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -3054,7 +3054,7 @@
         <v>45201</v>
       </c>
       <c r="G10" s="30">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H10" s="24"/>
       <c r="I10" s="34" t="str">
@@ -3297,11 +3297,11 @@
         <v>0</v>
       </c>
       <c r="F11" s="29">
-        <f>F10+14</f>
-        <v>45215</v>
+        <f>F10+21</f>
+        <v>45222</v>
       </c>
       <c r="G11" s="30">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H11" s="24"/>
       <c r="I11" s="34" t="str">
@@ -3544,11 +3544,11 @@
         <v>0</v>
       </c>
       <c r="F12" s="29">
-        <f t="shared" ref="F12:F15" si="10">F11+14</f>
-        <v>45229</v>
+        <f t="shared" ref="F12:F15" si="10">F11+21</f>
+        <v>45243</v>
       </c>
       <c r="G12" s="30">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H12" s="24"/>
       <c r="I12" s="34" t="str">
@@ -3792,10 +3792,10 @@
       </c>
       <c r="F13" s="29">
         <f t="shared" si="10"/>
-        <v>45243</v>
+        <v>45264</v>
       </c>
       <c r="G13" s="30">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H13" s="24"/>
       <c r="I13" s="34" t="str">
@@ -4039,10 +4039,10 @@
       </c>
       <c r="F14" s="29">
         <f t="shared" si="10"/>
-        <v>45257</v>
+        <v>45285</v>
       </c>
       <c r="G14" s="30">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H14" s="24"/>
       <c r="I14" s="34" t="str">
@@ -4286,10 +4286,10 @@
       </c>
       <c r="F15" s="29">
         <f t="shared" si="10"/>
-        <v>45271</v>
+        <v>45306</v>
       </c>
       <c r="G15" s="30">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H15" s="24"/>
       <c r="I15" s="34" t="str">

</xml_diff>